<commit_message>
added rake task and method for rolling over collection with timezone awareness
</commit_message>
<xml_diff>
--- a/aug_2018_rollover.xlsx
+++ b/aug_2018_rollover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FWallace/Shopify/new_rollover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F25CB7B1-B6B3-E942-B7D6-EDE52D2B0C6C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F44990C-00B9-0748-83C9-3C58C81B3579}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37380" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{3D7FB7DC-4E72-0841-96A1-B2D367058854}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{3D7FB7DC-4E72-0841-96A1-B2D367058854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>product_title</t>
   </si>
   <si>
-    <t>Print Paradise 3 Items</t>
-  </si>
-  <si>
     <t>new_title</t>
   </si>
   <si>
@@ -51,16 +48,19 @@
     <t>product.past-collection.bra</t>
   </si>
   <si>
-    <t>Seeing Stars 3 Items</t>
-  </si>
-  <si>
     <t>Seeing Stars (the July Collection 2018)</t>
   </si>
   <si>
-    <t>Vitamin Sea 3 Items</t>
-  </si>
-  <si>
     <t>Vitamin Sea (the July Collection 2018)</t>
+  </si>
+  <si>
+    <t>Meet Your Match 3 Items</t>
+  </si>
+  <si>
+    <t>Tough Luxe 3 Items</t>
+  </si>
+  <si>
+    <t>Power Surge 3 Items</t>
   </si>
 </sst>
 </file>
@@ -433,67 +433,67 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>1337218170972</v>
+        <v>1371333656668</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>49.95</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>1337218859100</v>
+        <v>1371334639708</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>49.95</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>1337219186780</v>
+        <v>1372047638620</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>49.95</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>